<commit_message>
discussion and results update
</commit_message>
<xml_diff>
--- a/Notes/litReview.xlsx
+++ b/Notes/litReview.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krtenneson\Desktop\lidarPaper\lidarNew\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\166.2.126.25\rseat\Programs\Reimbursibles\fy2016\R3_lidar_equation_transferability\Analysis\VersionControl\lidarNew\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="373">
   <si>
     <t>Model selection</t>
   </si>
@@ -3420,6 +3420,49 @@
   </si>
   <si>
     <t>plot; L-moment</t>
+  </si>
+  <si>
+    <r>
+      <t>Næsset, E., Gobakken, T., Solberg, S., Gregoire, T. G., Nelson, R., Ståhl, G., &amp; Weydahl, D. (2011). Model-assisted regional forest biomass estimation using LiDAR and InSAR as auxiliary data: a case study from a boreal forest area. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Remote Sensing of Environment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>115</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(12), 3599-3614.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3711,7 +3754,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3855,7 +3898,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3897,7 +3939,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3926,7 +3967,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3934,6 +3974,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4263,11 +4315,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC111"/>
+  <dimension ref="A1:AC113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC78" sqref="AC78"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC20" sqref="AC10:AC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4385,16 +4437,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" s="1" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
-      <c r="B2" t="s">
-        <v>251</v>
+      <c r="B2" s="51" t="s">
+        <v>162</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D2" s="2">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -4406,7 +4458,9 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="8"/>
+      <c r="M2" s="8" t="s">
+        <v>315</v>
+      </c>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
@@ -4416,50 +4470,46 @@
       <c r="T2" s="8"/>
       <c r="U2" s="9"/>
       <c r="V2" s="6"/>
-      <c r="W2" s="10"/>
+      <c r="W2" s="10" t="s">
+        <v>296</v>
+      </c>
       <c r="X2" s="10"/>
       <c r="Y2" s="10"/>
       <c r="Z2" s="10"/>
       <c r="AA2" s="10"/>
       <c r="AB2" s="10"/>
-      <c r="AC2" s="50" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D3" s="11">
-        <v>2012</v>
+      <c r="AC2" s="58" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="75"/>
+      <c r="B3" s="85" t="s">
+        <v>370</v>
+      </c>
+      <c r="C3" s="86" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="86">
+        <v>2014</v>
       </c>
       <c r="E3" s="11">
         <v>1</v>
       </c>
-      <c r="M3" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="W3" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="AC3" s="59" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4" t="s">
-        <v>281</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2015</v>
+      <c r="AC3" s="75" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="1" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="75"/>
+      <c r="B4" s="85" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" s="86" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="89">
+        <v>2014</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -4487,254 +4537,253 @@
       <c r="Z4" s="10"/>
       <c r="AA4" s="10"/>
       <c r="AB4" s="10"/>
-      <c r="AC4" s="50" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="D5" s="11">
-        <v>2003</v>
+      <c r="AC4" s="75" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="75"/>
+      <c r="B5" s="85" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" s="86" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="86">
+        <v>2015</v>
       </c>
       <c r="E5" s="11">
         <v>1</v>
       </c>
-      <c r="AC5" s="50" t="s">
-        <v>236</v>
+      <c r="AC5" s="75" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="88"/>
+      <c r="A6" s="87"/>
       <c r="B6" s="88" t="s">
-        <v>371</v>
-      </c>
-      <c r="C6" s="89" t="s">
-        <v>263</v>
-      </c>
-      <c r="D6" s="89">
-        <v>2011</v>
+        <v>370</v>
+      </c>
+      <c r="C6" s="86" t="s">
+        <v>369</v>
+      </c>
+      <c r="D6" s="86">
+        <v>2012</v>
       </c>
       <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="AC6" s="50" t="s">
-        <v>286</v>
+      <c r="AC6" s="87" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B7" s="55" t="s">
-        <v>264</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="38">
-        <v>2008</v>
-      </c>
-      <c r="E7" s="38">
+      <c r="A7" s="75"/>
+      <c r="B7" s="85" t="s">
+        <v>370</v>
+      </c>
+      <c r="C7" s="86" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="86">
+        <v>2014</v>
+      </c>
+      <c r="E7" s="11">
         <v>1</v>
       </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="38"/>
-      <c r="AC7" s="50" t="s">
-        <v>352</v>
+      <c r="AC7" s="87" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="77"/>
-      <c r="B8" s="88" t="s">
+      <c r="A8" s="75"/>
+      <c r="B8" s="85" t="s">
         <v>370</v>
       </c>
-      <c r="C8" s="89" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="89">
-        <v>2014</v>
+      <c r="C8" s="86" t="s">
+        <v>368</v>
+      </c>
+      <c r="D8" s="86">
+        <v>2016</v>
       </c>
       <c r="E8" s="11">
         <v>1</v>
       </c>
-      <c r="AC8" s="77" t="s">
-        <v>365</v>
+      <c r="AC8" s="87" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>264</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="D9" s="11">
-        <v>2015</v>
+      <c r="A9" s="75"/>
+      <c r="B9" s="85" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="86" t="s">
+        <v>367</v>
+      </c>
+      <c r="D9" s="86">
+        <v>2016</v>
       </c>
       <c r="E9" s="11">
         <v>1</v>
       </c>
-      <c r="AC9" s="50" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="77"/>
-      <c r="B10" s="88" t="s">
-        <v>370</v>
-      </c>
-      <c r="C10" s="89" t="s">
-        <v>265</v>
-      </c>
-      <c r="D10" s="89">
-        <v>2014</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="AC9" s="87" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B10" s="55" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="38">
+        <v>2008</v>
+      </c>
+      <c r="E10" s="38">
         <v>1</v>
       </c>
-      <c r="AC10" s="77" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="77"/>
-      <c r="B11" s="88" t="s">
-        <v>370</v>
-      </c>
-      <c r="C11" s="89" t="s">
-        <v>265</v>
-      </c>
-      <c r="D11" s="89">
+      <c r="G10" s="39"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="92" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>264</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" s="11">
         <v>2015</v>
       </c>
       <c r="E11" s="11">
         <v>1</v>
       </c>
-      <c r="AC11" s="77" t="s">
-        <v>363</v>
+      <c r="AC11" s="92" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="D12" s="11">
-        <v>2013</v>
+      <c r="A12" s="85"/>
+      <c r="B12" s="85" t="s">
+        <v>371</v>
+      </c>
+      <c r="C12" s="86" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" s="86">
+        <v>2011</v>
       </c>
       <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="AC12" s="50" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="AC12" s="92" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B13" s="38" t="s">
+        <v>191</v>
+      </c>
       <c r="C13" s="11" t="s">
-        <v>312</v>
+        <v>237</v>
       </c>
       <c r="D13" s="11">
-        <v>2013</v>
+        <v>2003</v>
       </c>
       <c r="E13" s="11">
         <v>1</v>
       </c>
-      <c r="M13" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="W13" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="AC13" s="50" t="s">
-        <v>318</v>
+      <c r="AC13" s="92" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="90"/>
-      <c r="B14" s="91" t="s">
-        <v>370</v>
-      </c>
-      <c r="C14" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="D14" s="89">
-        <v>2012</v>
+      <c r="A14" s="51"/>
+      <c r="B14" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="D14" s="11">
+        <v>2002</v>
       </c>
       <c r="E14" s="11">
         <v>1</v>
       </c>
-      <c r="AC14" s="90" t="s">
-        <v>364</v>
+      <c r="AC14" s="93" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="51"/>
-      <c r="B15" s="51" t="s">
-        <v>191</v>
+      <c r="B15" t="s">
+        <v>251</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>340</v>
+        <v>244</v>
       </c>
       <c r="D15" s="11">
-        <v>2002</v>
+        <v>2013</v>
       </c>
       <c r="E15" s="11">
         <v>1</v>
       </c>
-      <c r="AC15" s="59" t="s">
-        <v>339</v>
+      <c r="AC15" s="92" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
-      <c r="B16" s="88" t="s">
-        <v>370</v>
-      </c>
-      <c r="C16" s="89" t="s">
-        <v>214</v>
-      </c>
-      <c r="D16" s="89">
-        <v>2014</v>
+      <c r="A16" s="51"/>
+      <c r="B16" s="51" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2012</v>
       </c>
       <c r="E16" s="11">
         <v>1</v>
       </c>
-      <c r="AC16" s="90" t="s">
-        <v>366</v>
+      <c r="AC16" s="93" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="D17" s="2">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
@@ -4762,44 +4811,45 @@
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
       <c r="AB17" s="10"/>
-      <c r="AC17" s="57" t="s">
-        <v>253</v>
+      <c r="AC17" s="94" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
-      <c r="B18" s="88" t="s">
-        <v>370</v>
-      </c>
-      <c r="C18" s="89" t="s">
-        <v>368</v>
-      </c>
-      <c r="D18" s="89">
-        <v>2016</v>
+      <c r="B18" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" s="11">
+        <v>2013</v>
       </c>
       <c r="E18" s="11">
         <v>1</v>
       </c>
-      <c r="AC18" s="90" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="77"/>
-      <c r="B19" s="88" t="s">
-        <v>370</v>
-      </c>
-      <c r="C19" s="89" t="s">
-        <v>367</v>
-      </c>
-      <c r="D19" s="89">
-        <v>2016</v>
+      <c r="AC18" s="92" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2013</v>
       </c>
       <c r="E19" s="11">
         <v>1</v>
       </c>
-      <c r="AC19" s="90" t="s">
-        <v>361</v>
+      <c r="M19" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="W19" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC19" s="92" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -4812,7 +4862,7 @@
       <c r="E20" s="11">
         <v>1</v>
       </c>
-      <c r="AC20" s="50" t="s">
+      <c r="AC20" s="92" t="s">
         <v>239</v>
       </c>
     </row>
@@ -5032,702 +5082,703 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="96.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="51"/>
-      <c r="B25" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="38">
-        <v>2002</v>
-      </c>
-      <c r="E25" s="38" t="s">
+    <row r="25" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="73">
+        <v>43101</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D25" s="11">
+        <v>2008</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="G25" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H25" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="I25" s="40" t="s">
-        <v>323</v>
-      </c>
-      <c r="J25" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="K25" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="L25" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="M25" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="V25" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="X25" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y25" s="38">
-        <v>5</v>
-      </c>
-      <c r="Z25" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA25" s="38"/>
-      <c r="AB25" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC25" s="56" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="74">
-        <v>43101</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="38">
-        <v>2005</v>
-      </c>
-      <c r="E26" s="38" t="s">
+      <c r="F25" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="17">
+        <v>3</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="P25" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="S25" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="T25" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="U25" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="X25" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y25" s="21">
+        <v>6</v>
+      </c>
+      <c r="Z25" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="AB25" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC25" s="52" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="51"/>
+      <c r="B26" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2004</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="G26" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="H26" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="I26" s="40" t="s">
-        <v>323</v>
-      </c>
-      <c r="J26" s="38"/>
-      <c r="K26" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="L26" s="39"/>
-      <c r="M26" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
+      <c r="G26" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="17">
+        <v>1000</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="M26" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="O26" s="19" t="s">
+        <v>95</v>
+      </c>
       <c r="S26" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="T26" s="38"/>
-      <c r="U26" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="V26" s="38"/>
-      <c r="X26" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y26" s="38" t="s">
+      <c r="T26" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="U26" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="X26" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y26" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC26" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="73">
+        <v>43113</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D27" s="11">
+        <v>2017</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="J27" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="Z26" s="38">
-        <v>0.92</v>
-      </c>
-      <c r="AA26" s="38"/>
-      <c r="AB26" s="38"/>
-      <c r="AC26" s="56" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="74">
-        <v>43101</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="38">
-        <v>2005</v>
-      </c>
-      <c r="E27" s="38" t="s">
-        <v>260</v>
-      </c>
-      <c r="G27" s="39"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="L27" s="39"/>
-      <c r="M27" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="40"/>
-      <c r="V27" s="38"/>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38"/>
-      <c r="Z27" s="38"/>
-      <c r="AA27" s="38"/>
-      <c r="AB27" s="38"/>
-      <c r="AC27" s="56" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="74">
-        <v>43101</v>
-      </c>
-      <c r="B28" s="51" t="s">
+      <c r="K27" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="M27" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="O27" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="P27" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q27" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="S27" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="T27" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="U27" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="V27" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="W27" s="21">
+        <v>100.5</v>
+      </c>
+      <c r="X27" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y27" s="21">
+        <v>9</v>
+      </c>
+      <c r="Z27" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="AB27" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="AC27" s="58" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="108.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="38" t="s">
         <v>162</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="D28" s="11">
-        <v>2008</v>
+        <v>2015</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>260</v>
       </c>
       <c r="F28" s="46" t="s">
-        <v>229</v>
+        <v>345</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>215</v>
+        <v>341</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>216</v>
+        <v>342</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J28" s="17">
+        <v>323</v>
+      </c>
+      <c r="J28" s="74">
+        <v>189000</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="N28" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="O28" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q28" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="T28" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="U28" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="V28" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="W28" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="X28" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="Y28" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="Z28" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA28" s="21">
         <v>3</v>
       </c>
-      <c r="K28" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="M28" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="O28" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="P28" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q28" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="S28" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="T28" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="U28" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="X28" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y28" s="21">
-        <v>6</v>
-      </c>
-      <c r="Z28" s="21">
-        <v>0.75</v>
-      </c>
-      <c r="AB28" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="AC28" s="52" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="51"/>
+      <c r="AC28" s="50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="60">
+        <v>43101</v>
+      </c>
       <c r="B29" s="51" t="s">
         <v>162</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="D29" s="11">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>260</v>
       </c>
+      <c r="F29" s="46" t="s">
+        <v>211</v>
+      </c>
       <c r="G29" s="14" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J29" s="17">
-        <v>1000</v>
+        <v>323</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="M29" s="19" t="s">
         <v>83</v>
       </c>
       <c r="O29" s="19" t="s">
-        <v>95</v>
+        <v>123</v>
+      </c>
+      <c r="Q29" s="19" t="s">
+        <v>122</v>
       </c>
       <c r="S29" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="T29" s="19" t="s">
-        <v>97</v>
-      </c>
       <c r="U29" s="20" t="s">
-        <v>93</v>
+        <v>225</v>
+      </c>
+      <c r="V29" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="X29" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y29" s="21">
-        <v>1</v>
-      </c>
-      <c r="Z29" s="21" t="s">
-        <v>96</v>
+        <v>124</v>
+      </c>
+      <c r="Y29" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z29" s="21">
+        <v>0.92</v>
       </c>
       <c r="AC29" s="24" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="74">
-        <v>43113</v>
-      </c>
-      <c r="B30" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>233</v>
+      <c r="A30" s="60">
+        <v>43101</v>
+      </c>
+      <c r="B30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>6</v>
       </c>
       <c r="D30" s="11">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>260</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>290</v>
+        <v>42</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>291</v>
+        <v>25</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>292</v>
+        <v>43</v>
+      </c>
+      <c r="J30" s="17">
+        <v>1000</v>
+      </c>
+      <c r="K30" s="17">
+        <v>144</v>
       </c>
       <c r="L30" s="18" t="s">
-        <v>305</v>
+        <v>36</v>
       </c>
       <c r="M30" s="19" t="s">
-        <v>297</v>
+        <v>61</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="P30" s="19" t="s">
-        <v>299</v>
+        <v>31</v>
       </c>
       <c r="Q30" s="19" t="s">
-        <v>298</v>
+        <v>32</v>
       </c>
       <c r="S30" s="19" t="s">
-        <v>294</v>
+        <v>333</v>
       </c>
       <c r="T30" s="19" t="s">
-        <v>306</v>
+        <v>33</v>
       </c>
       <c r="U30" s="20" t="s">
-        <v>307</v>
+        <v>28</v>
       </c>
       <c r="V30" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="W30" s="21">
-        <v>100.5</v>
+        <v>27</v>
       </c>
       <c r="X30" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="Y30" s="21">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="Y30" s="21" t="s">
+        <v>44</v>
       </c>
       <c r="Z30" s="21" t="s">
-        <v>311</v>
+        <v>39</v>
       </c>
       <c r="AB30" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="AC30" s="59" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="61">
-        <v>43101</v>
-      </c>
-      <c r="B31" t="s">
-        <v>192</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>6</v>
+        <v>40</v>
+      </c>
+      <c r="AC30" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="73">
+        <v>43113</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>234</v>
       </c>
       <c r="D31" s="11">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>260</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>42</v>
+        <v>290</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>25</v>
+        <v>322</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J31" s="17">
-        <v>1000</v>
-      </c>
-      <c r="K31" s="17">
-        <v>144</v>
-      </c>
-      <c r="L31" s="18" t="s">
-        <v>36</v>
+        <v>302</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>325</v>
       </c>
       <c r="M31" s="19" t="s">
-        <v>61</v>
+        <v>324</v>
+      </c>
+      <c r="N31" s="19" t="s">
+        <v>347</v>
       </c>
       <c r="O31" s="19" t="s">
-        <v>30</v>
+        <v>348</v>
       </c>
       <c r="P31" s="19" t="s">
-        <v>31</v>
+        <v>349</v>
       </c>
       <c r="Q31" s="19" t="s">
-        <v>32</v>
+        <v>326</v>
+      </c>
+      <c r="R31" s="19" t="s">
+        <v>329</v>
       </c>
       <c r="S31" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="T31" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="U31" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="V31" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="X31" s="21">
+        <v>2</v>
+      </c>
+      <c r="Y31" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z31" s="21">
+        <v>0.81</v>
+      </c>
+      <c r="AA31" s="21">
+        <v>12</v>
+      </c>
+      <c r="AB31" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="AC31" s="58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="96.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="51"/>
+      <c r="B32" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="38">
+        <v>2002</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="G32" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="40" t="s">
+        <v>323</v>
+      </c>
+      <c r="J32" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="K32" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="M32" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="R32" s="38"/>
+      <c r="S32" s="38"/>
+      <c r="T32" s="38"/>
+      <c r="U32" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="V32" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="X32" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y32" s="38">
+        <v>5</v>
+      </c>
+      <c r="Z32" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA32" s="38"/>
+      <c r="AB32" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC32" s="56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="73">
+        <v>43101</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="38">
+        <v>2005</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="G33" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="40" t="s">
+        <v>323</v>
+      </c>
+      <c r="J33" s="38"/>
+      <c r="K33" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="L33" s="39"/>
+      <c r="M33" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
+      <c r="S33" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="T31" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="U31" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="V31" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="X31" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y31" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z31" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB31" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC31" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="74">
-        <v>43113</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="D32" s="11">
-        <v>2017</v>
-      </c>
-      <c r="E32" s="11" t="s">
+      <c r="T33" s="38"/>
+      <c r="U33" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="V33" s="38"/>
+      <c r="X33" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y33" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z33" s="38">
+        <v>0.92</v>
+      </c>
+      <c r="AA33" s="38"/>
+      <c r="AB33" s="38"/>
+      <c r="AC33" s="56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="73">
+        <v>43101</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="38">
+        <v>2005</v>
+      </c>
+      <c r="E34" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="G32" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="K32" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="M32" s="19" t="s">
-        <v>324</v>
-      </c>
-      <c r="N32" s="19" t="s">
-        <v>347</v>
-      </c>
-      <c r="O32" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="P32" s="19" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q32" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="R32" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="S32" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="T32" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="U32" s="20" t="s">
-        <v>330</v>
-      </c>
-      <c r="V32" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="X32" s="21">
-        <v>2</v>
-      </c>
-      <c r="Y32" s="21" t="s">
-        <v>332</v>
-      </c>
-      <c r="Z32" s="21">
-        <v>0.81</v>
-      </c>
-      <c r="AA32" s="21">
-        <v>12</v>
-      </c>
-      <c r="AB32" s="21" t="s">
-        <v>328</v>
-      </c>
-      <c r="AC32" s="59" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" ht="108.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="D33" s="11">
-        <v>2015</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F33" s="46" t="s">
-        <v>345</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="J33" s="76">
-        <v>189000</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>351</v>
-      </c>
-      <c r="L33" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="M33" s="19" t="s">
-        <v>343</v>
-      </c>
-      <c r="N33" s="19" t="s">
-        <v>350</v>
-      </c>
-      <c r="O33" s="19" t="s">
-        <v>353</v>
-      </c>
-      <c r="Q33" s="19" t="s">
-        <v>354</v>
-      </c>
-      <c r="T33" s="19" t="s">
-        <v>357</v>
-      </c>
-      <c r="U33" s="20" t="s">
-        <v>356</v>
-      </c>
-      <c r="V33" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="W33" s="21" t="s">
-        <v>344</v>
-      </c>
-      <c r="X33" s="21" t="s">
-        <v>358</v>
-      </c>
-      <c r="Y33" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="Z33" s="21" t="s">
-        <v>360</v>
-      </c>
-      <c r="AA33" s="21">
-        <v>3</v>
-      </c>
-      <c r="AC33" s="50" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="61">
-        <v>43101</v>
-      </c>
-      <c r="B34" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="11">
-        <v>2008</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F34" s="46" t="s">
-        <v>211</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="L34" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="M34" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="O34" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q34" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="S34" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="U34" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="V34" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="X34" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y34" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z34" s="21">
-        <v>0.92</v>
-      </c>
-      <c r="AC34" s="24" t="s">
-        <v>109</v>
+      <c r="G34" s="39"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="L34" s="39"/>
+      <c r="M34" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="38"/>
+      <c r="S34" s="38"/>
+      <c r="T34" s="38"/>
+      <c r="U34" s="40"/>
+      <c r="V34" s="38"/>
+      <c r="X34" s="38"/>
+      <c r="Y34" s="38"/>
+      <c r="Z34" s="38"/>
+      <c r="AA34" s="38"/>
+      <c r="AB34" s="38"/>
+      <c r="AC34" s="56" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="51"/>
-      <c r="B35" s="51"/>
+      <c r="B35" t="s">
+        <v>162</v>
+      </c>
       <c r="C35" s="11" t="s">
-        <v>244</v>
+        <v>163</v>
       </c>
       <c r="D35" s="11">
-        <v>2013</v>
-      </c>
-      <c r="AC35" s="59" t="s">
-        <v>249</v>
+        <v>2009</v>
+      </c>
+      <c r="AC35" s="23" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
       <c r="B36" t="s">
         <v>162</v>
       </c>
@@ -5735,10 +5786,10 @@
         <v>163</v>
       </c>
       <c r="D36" s="11">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="AC36" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
@@ -5752,7 +5803,7 @@
         <v>2010</v>
       </c>
       <c r="AC37" s="23" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
@@ -5763,10 +5814,10 @@
         <v>163</v>
       </c>
       <c r="D38" s="11">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="AC38" s="23" t="s">
-        <v>193</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
@@ -5777,10 +5828,10 @@
         <v>163</v>
       </c>
       <c r="D39" s="11">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="AC39" s="23" t="s">
-        <v>129</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
@@ -5794,7 +5845,7 @@
         <v>2012</v>
       </c>
       <c r="AC40" s="23" t="s">
-        <v>194</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
@@ -5808,7 +5859,7 @@
         <v>2012</v>
       </c>
       <c r="AC41" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
@@ -5816,13 +5867,13 @@
         <v>162</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D42" s="11">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="AC42" s="23" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
@@ -5830,13 +5881,13 @@
         <v>162</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D43" s="11">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="AC43" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.25">
@@ -5844,13 +5895,13 @@
         <v>162</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="D44" s="11">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="AC44" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
@@ -5858,13 +5909,13 @@
         <v>162</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D45" s="11">
-        <v>2012</v>
+        <v>2005</v>
       </c>
       <c r="AC45" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
@@ -5872,77 +5923,69 @@
         <v>162</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D46" s="11">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="AC46" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="A47" s="51"/>
+      <c r="B47" s="51" t="s">
         <v>162</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D47" s="11">
-        <v>2008</v>
-      </c>
-      <c r="AC47" s="23" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
+        <v>2011</v>
+      </c>
+      <c r="AC47" s="52" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
       <c r="B48" s="51" t="s">
-        <v>316</v>
+        <v>162</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>313</v>
+        <v>173</v>
       </c>
       <c r="D48" s="11">
-        <v>2014</v>
-      </c>
-      <c r="M48" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="W48" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="AC48" s="59" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="49" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
+        <v>2012</v>
+      </c>
+      <c r="AC48" s="52" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
       <c r="B49" s="51" t="s">
-        <v>316</v>
+        <v>162</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>313</v>
+        <v>169</v>
       </c>
       <c r="D49" s="11">
-        <v>2014</v>
-      </c>
-      <c r="M49" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="W49" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="AC49" s="59" t="s">
-        <v>319</v>
+        <v>2009</v>
+      </c>
+      <c r="AC49" s="52" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="C50" s="2" t="s">
-        <v>245</v>
+        <v>172</v>
       </c>
       <c r="D50" s="2">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="45"/>
@@ -5968,8 +6011,8 @@
       <c r="Z50" s="10"/>
       <c r="AA50" s="10"/>
       <c r="AB50" s="10"/>
-      <c r="AC50" s="57" t="s">
-        <v>254</v>
+      <c r="AC50" s="48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5977,10 +6020,10 @@
         <v>162</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D51" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="45"/>
@@ -6007,54 +6050,57 @@
       <c r="AA51" s="10"/>
       <c r="AB51" s="10"/>
       <c r="AC51" s="48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:29" s="72" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="D52" s="62">
-        <v>2011</v>
-      </c>
-      <c r="E52" s="62"/>
-      <c r="F52" s="63"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="65"/>
-      <c r="I52" s="66"/>
-      <c r="J52" s="67"/>
-      <c r="K52" s="67"/>
-      <c r="L52" s="68"/>
-      <c r="M52" s="69"/>
-      <c r="N52" s="69"/>
-      <c r="O52" s="69"/>
-      <c r="P52" s="69"/>
-      <c r="Q52" s="69"/>
-      <c r="R52" s="69"/>
-      <c r="S52" s="69"/>
-      <c r="T52" s="69"/>
-      <c r="U52" s="70"/>
-      <c r="V52" s="67"/>
-      <c r="W52" s="71"/>
-      <c r="X52" s="71"/>
-      <c r="Y52" s="71"/>
-      <c r="Z52" s="71"/>
-      <c r="AA52" s="71"/>
-      <c r="AB52" s="71"/>
-      <c r="AC52" s="75" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:29" s="60" customFormat="1" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="61">
+        <v>2010</v>
+      </c>
+      <c r="E52" s="61"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="64"/>
+      <c r="I52" s="65"/>
+      <c r="J52" s="66"/>
+      <c r="K52" s="66"/>
+      <c r="L52" s="67"/>
+      <c r="M52" s="68"/>
+      <c r="N52" s="68"/>
+      <c r="O52" s="68"/>
+      <c r="P52" s="68"/>
+      <c r="Q52" s="68"/>
+      <c r="R52" s="68"/>
+      <c r="S52" s="68"/>
+      <c r="T52" s="68"/>
+      <c r="U52" s="69"/>
+      <c r="V52" s="66"/>
+      <c r="W52" s="70"/>
+      <c r="X52" s="70"/>
+      <c r="Y52" s="70"/>
+      <c r="Z52" s="70"/>
+      <c r="AA52" s="70"/>
+      <c r="AB52" s="70"/>
+      <c r="AC52" s="91" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
       <c r="B53" s="51" t="s">
         <v>162</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D53" s="11">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="46"/>
@@ -6081,23 +6127,21 @@
       <c r="AA53" s="21"/>
       <c r="AB53" s="21"/>
       <c r="AC53" s="52" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>271</v>
+        <v>162</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>261</v>
+        <v>115</v>
       </c>
       <c r="D54" s="2">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="E54" s="2"/>
-      <c r="F54" s="45" t="s">
-        <v>285</v>
-      </c>
+      <c r="F54" s="45"/>
       <c r="G54" s="3"/>
       <c r="H54" s="4"/>
       <c r="I54" s="5"/>
@@ -6120,38 +6164,37 @@
       <c r="Z54" s="10"/>
       <c r="AA54" s="10"/>
       <c r="AB54" s="10"/>
-      <c r="AC54" s="57" t="s">
-        <v>284</v>
+      <c r="AC54" s="84" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="51"/>
       <c r="B55" s="51" t="s">
-        <v>264</v>
+        <v>162</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>268</v>
+        <v>177</v>
       </c>
       <c r="D55" s="11">
         <v>2011</v>
       </c>
-      <c r="AC55" s="59" t="s">
-        <v>288</v>
+      <c r="AC55" s="52" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A56" s="51"/>
-      <c r="B56" s="51" t="s">
+      <c r="B56" t="s">
         <v>162</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="D56" s="11">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="AC56" s="52" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6159,10 +6202,10 @@
         <v>162</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D57" s="2">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="45"/>
@@ -6189,138 +6232,118 @@
       <c r="AA57" s="10"/>
       <c r="AB57" s="10"/>
       <c r="AC57" s="23" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" s="51"/>
-      <c r="B58" s="55" t="s">
-        <v>189</v>
-      </c>
-      <c r="C58" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="D58" s="38">
+      <c r="B58" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D58" s="11">
+        <v>2011</v>
+      </c>
+      <c r="AC58" s="52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59" s="11">
+        <v>2011</v>
+      </c>
+      <c r="AC59" s="23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="11">
+        <v>2007</v>
+      </c>
+      <c r="AC60" s="52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="11">
         <v>2012</v>
       </c>
-      <c r="E58" s="38"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="38"/>
-      <c r="N58" s="38"/>
-      <c r="O58" s="38"/>
-      <c r="P58" s="38"/>
-      <c r="Q58" s="38"/>
-      <c r="R58" s="38"/>
-      <c r="S58" s="38"/>
-      <c r="T58" s="38"/>
-      <c r="U58" s="40"/>
-      <c r="V58" s="38"/>
-      <c r="X58" s="38"/>
-      <c r="Y58" s="38"/>
-      <c r="Z58" s="38"/>
-      <c r="AA58" s="38"/>
-      <c r="AB58" s="38"/>
-      <c r="AC58" s="53" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A59" s="51"/>
-      <c r="B59" s="51" t="s">
+      <c r="AC61" s="52" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>162</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D59" s="11">
+      <c r="C62" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D62" s="11">
         <v>2012</v>
       </c>
-      <c r="AC59" s="52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A60" s="51"/>
-      <c r="B60" s="51" t="s">
+      <c r="AC62" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>162</v>
       </c>
-      <c r="C60" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="11">
-        <v>2010</v>
-      </c>
-      <c r="AC60" s="52" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A61" s="51"/>
-      <c r="B61" s="51" t="s">
+      <c r="C63" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D63" s="11">
+        <v>2004</v>
+      </c>
+      <c r="AC63" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D61" s="11">
-        <v>2009</v>
-      </c>
-      <c r="AC61" s="52" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C62" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="D62" s="11">
-        <v>2013</v>
-      </c>
-      <c r="AC62" s="50" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A63" s="51"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="D63" s="11">
-        <v>2009</v>
-      </c>
-      <c r="AC63" s="59" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A64" s="51"/>
-      <c r="B64" s="51"/>
       <c r="C64" s="11" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
       <c r="D64" s="11">
-        <v>2009</v>
-      </c>
-      <c r="AC64" s="59" t="s">
-        <v>213</v>
+        <v>2012</v>
+      </c>
+      <c r="AC64" s="23" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="51"/>
-      <c r="B65" s="51" t="s">
+      <c r="A65"/>
+      <c r="B65" t="s">
         <v>162</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D65" s="2">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="45"/>
@@ -6346,59 +6369,59 @@
       <c r="Z65" s="10"/>
       <c r="AA65" s="10"/>
       <c r="AB65" s="10"/>
-      <c r="AC65" s="87" t="s">
-        <v>111</v>
+      <c r="AC65" s="84" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="51"/>
-      <c r="B66" s="51" t="s">
-        <v>335</v>
-      </c>
-      <c r="C66" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="D66" s="78">
+      <c r="A66"/>
+      <c r="B66" t="s">
+        <v>162</v>
+      </c>
+      <c r="C66" s="76" t="s">
+        <v>117</v>
+      </c>
+      <c r="D66" s="76">
         <v>2007</v>
       </c>
-      <c r="E66" s="78"/>
+      <c r="E66" s="76"/>
       <c r="F66" s="47"/>
-      <c r="G66" s="79"/>
-      <c r="H66" s="80"/>
-      <c r="I66" s="81"/>
-      <c r="J66" s="82"/>
+      <c r="G66" s="77"/>
+      <c r="H66" s="78"/>
+      <c r="I66" s="79"/>
+      <c r="J66" s="80"/>
       <c r="K66" s="17"/>
-      <c r="L66" s="83"/>
+      <c r="L66" s="81"/>
       <c r="M66" s="8"/>
-      <c r="N66" s="84"/>
-      <c r="O66" s="84"/>
-      <c r="P66" s="84"/>
-      <c r="Q66" s="84"/>
-      <c r="R66" s="84"/>
-      <c r="S66" s="84"/>
-      <c r="T66" s="84"/>
-      <c r="U66" s="85"/>
-      <c r="V66" s="82"/>
-      <c r="W66" s="73"/>
-      <c r="X66" s="73"/>
-      <c r="Y66" s="73"/>
-      <c r="Z66" s="73"/>
-      <c r="AA66" s="73"/>
-      <c r="AB66" s="73"/>
-      <c r="AC66" s="86" t="s">
-        <v>338</v>
+      <c r="N66" s="82"/>
+      <c r="O66" s="82"/>
+      <c r="P66" s="82"/>
+      <c r="Q66" s="82"/>
+      <c r="R66" s="82"/>
+      <c r="S66" s="82"/>
+      <c r="T66" s="82"/>
+      <c r="U66" s="83"/>
+      <c r="V66" s="80"/>
+      <c r="W66" s="72"/>
+      <c r="X66" s="72"/>
+      <c r="Y66" s="72"/>
+      <c r="Z66" s="72"/>
+      <c r="AA66" s="72"/>
+      <c r="AB66" s="72"/>
+      <c r="AC66" s="90" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="51"/>
-      <c r="B67" s="51" t="s">
+      <c r="A67"/>
+      <c r="B67" t="s">
         <v>162</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D67" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="45"/>
@@ -6425,7 +6448,7 @@
       <c r="AA67" s="10"/>
       <c r="AB67" s="10"/>
       <c r="AC67" s="48" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6434,7 +6457,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="D68" s="2">
         <v>2008</v>
@@ -6464,17 +6487,19 @@
       <c r="AA68" s="10"/>
       <c r="AB68" s="10"/>
       <c r="AC68" s="48" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="51"/>
-      <c r="B69" s="51"/>
+      <c r="A69"/>
+      <c r="B69" t="s">
+        <v>162</v>
+      </c>
       <c r="C69" s="2" t="s">
-        <v>247</v>
+        <v>118</v>
       </c>
       <c r="D69" s="2">
-        <v>2012</v>
+        <v>2006</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="45"/>
@@ -6500,36 +6525,36 @@
       <c r="Z69" s="10"/>
       <c r="AA69" s="10"/>
       <c r="AB69" s="10"/>
-      <c r="AC69" s="57" t="s">
-        <v>255</v>
+      <c r="AC69" s="84" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A70" s="51"/>
-      <c r="B70" s="51" t="s">
-        <v>271</v>
+      <c r="B70" t="s">
+        <v>162</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>283</v>
+        <v>188</v>
       </c>
       <c r="D70" s="11">
-        <v>2014</v>
-      </c>
-      <c r="AC70" s="50" t="s">
-        <v>282</v>
+        <v>2012</v>
+      </c>
+      <c r="AC70" s="23" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A71" s="60"/>
-      <c r="B71" s="51"/>
+      <c r="B71" t="s">
+        <v>162</v>
+      </c>
       <c r="C71" s="11" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="D71" s="11">
-        <v>2015</v>
-      </c>
-      <c r="AC71" s="59" t="s">
-        <v>259</v>
+        <v>2006</v>
+      </c>
+      <c r="AC71" s="23" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.25">
@@ -6537,309 +6562,177 @@
         <v>162</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="D72" s="11">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="AC72" s="23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A73" s="51"/>
       <c r="B73" s="51" t="s">
-        <v>162</v>
+        <v>316</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>181</v>
+        <v>313</v>
       </c>
       <c r="D73" s="11">
-        <v>2011</v>
-      </c>
-      <c r="AC73" s="52" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>264</v>
+        <v>2014</v>
+      </c>
+      <c r="M73" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="W73" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC73" s="58" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="51"/>
+      <c r="B74" s="51" t="s">
+        <v>316</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>266</v>
+        <v>313</v>
       </c>
       <c r="D74" s="11">
-        <v>2015</v>
-      </c>
-      <c r="AC74" s="59" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B75" s="37" t="s">
+        <v>2014</v>
+      </c>
+      <c r="M74" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="W74" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC74" s="58" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>316</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="D75" s="11">
+        <v>2014</v>
+      </c>
+      <c r="M75" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="W75" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC75" s="50" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A76" s="51"/>
+      <c r="B76" s="51" t="s">
+        <v>335</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D76" s="11">
+        <v>2007</v>
+      </c>
+      <c r="AC76" s="58" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>335</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="D77" s="11">
+        <v>2009</v>
+      </c>
+      <c r="AC77" s="50" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A78" s="51"/>
+      <c r="B78" s="51" t="s">
+        <v>271</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D78" s="11">
+        <v>2014</v>
+      </c>
+      <c r="F78" s="46" t="s">
+        <v>285</v>
+      </c>
+      <c r="AC78" s="58" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A79" s="51"/>
+      <c r="B79" s="51" t="s">
+        <v>271</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="D79" s="11">
+        <v>2014</v>
+      </c>
+      <c r="AC79" s="50" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>271</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D80" s="11">
+        <v>2014</v>
+      </c>
+      <c r="AC80" s="50" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>271</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D81" s="11">
+        <v>2012</v>
+      </c>
+      <c r="AC81" s="50" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A82" s="51"/>
+      <c r="B82" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="C75" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="38">
-        <v>1997</v>
-      </c>
-      <c r="E75" s="38"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="38"/>
-      <c r="I75" s="40"/>
-      <c r="J75" s="38"/>
-      <c r="K75" s="38"/>
-      <c r="L75" s="39"/>
-      <c r="M75" s="38"/>
-      <c r="N75" s="38"/>
-      <c r="O75" s="38"/>
-      <c r="P75" s="38"/>
-      <c r="Q75" s="38"/>
-      <c r="R75" s="38"/>
-      <c r="S75" s="38"/>
-      <c r="T75" s="38"/>
-      <c r="U75" s="40"/>
-      <c r="V75" s="38"/>
-      <c r="X75" s="38"/>
-      <c r="Y75" s="38"/>
-      <c r="Z75" s="38"/>
-      <c r="AA75" s="38"/>
-      <c r="AB75" s="38"/>
-      <c r="AC75" s="41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B76" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="C76" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="38">
-        <v>1997</v>
-      </c>
-      <c r="E76" s="38"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="38"/>
-      <c r="I76" s="40"/>
-      <c r="J76" s="38"/>
-      <c r="K76" s="38"/>
-      <c r="L76" s="39"/>
-      <c r="M76" s="38"/>
-      <c r="N76" s="38"/>
-      <c r="O76" s="38"/>
-      <c r="P76" s="38"/>
-      <c r="Q76" s="38"/>
-      <c r="R76" s="38"/>
-      <c r="S76" s="38"/>
-      <c r="T76" s="38"/>
-      <c r="U76" s="40"/>
-      <c r="V76" s="38"/>
-      <c r="X76" s="38"/>
-      <c r="Y76" s="38"/>
-      <c r="Z76" s="38"/>
-      <c r="AA76" s="38"/>
-      <c r="AB76" s="38"/>
-      <c r="AC76" s="41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B77" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="C77" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="38">
-        <v>2001</v>
-      </c>
-      <c r="E77" s="38"/>
-      <c r="G77" s="39"/>
-      <c r="H77" s="38"/>
-      <c r="I77" s="40"/>
-      <c r="J77" s="38"/>
-      <c r="K77" s="38"/>
-      <c r="L77" s="39"/>
-      <c r="M77" s="38"/>
-      <c r="N77" s="38"/>
-      <c r="O77" s="38"/>
-      <c r="P77" s="38"/>
-      <c r="Q77" s="38"/>
-      <c r="R77" s="38"/>
-      <c r="S77" s="38"/>
-      <c r="T77" s="38"/>
-      <c r="U77" s="40"/>
-      <c r="V77" s="38"/>
-      <c r="X77" s="38"/>
-      <c r="Y77" s="38"/>
-      <c r="Z77" s="38"/>
-      <c r="AA77" s="38"/>
-      <c r="AB77" s="38"/>
-      <c r="AC77" s="41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B78" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="C78" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="38">
-        <v>2004</v>
-      </c>
-      <c r="E78" s="38"/>
-      <c r="G78" s="39"/>
-      <c r="H78" s="38"/>
-      <c r="I78" s="40"/>
-      <c r="J78" s="38"/>
-      <c r="K78" s="38"/>
-      <c r="L78" s="39"/>
-      <c r="M78" s="38"/>
-      <c r="N78" s="38"/>
-      <c r="O78" s="38"/>
-      <c r="P78" s="38"/>
-      <c r="Q78" s="38"/>
-      <c r="R78" s="38"/>
-      <c r="S78" s="38"/>
-      <c r="T78" s="38"/>
-      <c r="U78" s="40"/>
-      <c r="V78" s="38"/>
-      <c r="X78" s="38"/>
-      <c r="Y78" s="38"/>
-      <c r="Z78" s="38"/>
-      <c r="AA78" s="38"/>
-      <c r="AB78" s="38"/>
-      <c r="AC78" s="41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:29" ht="24" x14ac:dyDescent="0.25">
-      <c r="A79" s="51"/>
-      <c r="B79" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="C79" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="38">
-        <v>2004</v>
-      </c>
-      <c r="E79" s="38"/>
-      <c r="G79" s="39"/>
-      <c r="H79" s="38"/>
-      <c r="I79" s="40"/>
-      <c r="J79" s="38"/>
-      <c r="K79" s="38"/>
-      <c r="L79" s="39"/>
-      <c r="M79" s="38"/>
-      <c r="N79" s="38"/>
-      <c r="O79" s="38"/>
-      <c r="P79" s="38"/>
-      <c r="Q79" s="38"/>
-      <c r="R79" s="38"/>
-      <c r="S79" s="38"/>
-      <c r="T79" s="38"/>
-      <c r="U79" s="40"/>
-      <c r="V79" s="38"/>
-      <c r="X79" s="38"/>
-      <c r="Y79" s="38"/>
-      <c r="Z79" s="38"/>
-      <c r="AA79" s="38"/>
-      <c r="AB79" s="38"/>
-      <c r="AC79" s="41" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80" spans="1:29" ht="24" x14ac:dyDescent="0.25">
-      <c r="A80" s="51"/>
-      <c r="B80" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="C80" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="38">
-        <v>2004</v>
-      </c>
-      <c r="E80" s="38"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="38"/>
-      <c r="I80" s="40"/>
-      <c r="J80" s="38"/>
-      <c r="K80" s="38"/>
-      <c r="L80" s="39"/>
-      <c r="M80" s="38"/>
-      <c r="N80" s="38"/>
-      <c r="O80" s="38"/>
-      <c r="P80" s="38"/>
-      <c r="Q80" s="38"/>
-      <c r="R80" s="38"/>
-      <c r="S80" s="38"/>
-      <c r="T80" s="38"/>
-      <c r="U80" s="40"/>
-      <c r="V80" s="38"/>
-      <c r="X80" s="38"/>
-      <c r="Y80" s="38"/>
-      <c r="Z80" s="38"/>
-      <c r="AA80" s="38"/>
-      <c r="AB80" s="38"/>
-      <c r="AC80" s="41" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" spans="1:29" ht="24" x14ac:dyDescent="0.25">
-      <c r="A81" s="51"/>
-      <c r="B81" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="C81" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="38">
-        <v>2005</v>
-      </c>
-      <c r="E81" s="38"/>
-      <c r="G81" s="39"/>
-      <c r="H81" s="38"/>
-      <c r="I81" s="40"/>
-      <c r="J81" s="38"/>
-      <c r="K81" s="38"/>
-      <c r="L81" s="39"/>
-      <c r="M81" s="38"/>
-      <c r="N81" s="38"/>
-      <c r="O81" s="38"/>
-      <c r="P81" s="38"/>
-      <c r="Q81" s="38"/>
-      <c r="R81" s="38"/>
-      <c r="S81" s="38"/>
-      <c r="T81" s="38"/>
-      <c r="U81" s="40"/>
-      <c r="V81" s="38"/>
-      <c r="X81" s="38"/>
-      <c r="Y81" s="38"/>
-      <c r="Z81" s="38"/>
-      <c r="AA81" s="38"/>
-      <c r="AB81" s="38"/>
-      <c r="AC81" s="41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="82" spans="1:29" ht="24" x14ac:dyDescent="0.25">
-      <c r="A82" s="51"/>
-      <c r="B82" s="37" t="s">
-        <v>189</v>
-      </c>
       <c r="C82" s="38" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="D82" s="38">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="E82" s="38"/>
       <c r="G82" s="39"/>
@@ -6863,12 +6756,11 @@
       <c r="Z82" s="38"/>
       <c r="AA82" s="38"/>
       <c r="AB82" s="38"/>
-      <c r="AC82" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="83" spans="1:29" ht="24" x14ac:dyDescent="0.25">
-      <c r="A83" s="51"/>
+      <c r="AC82" s="53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B83" s="37" t="s">
         <v>189</v>
       </c>
@@ -6876,7 +6768,7 @@
         <v>6</v>
       </c>
       <c r="D83" s="38">
-        <v>2009</v>
+        <v>1997</v>
       </c>
       <c r="E83" s="38"/>
       <c r="G83" s="39"/>
@@ -6901,10 +6793,10 @@
       <c r="AA83" s="38"/>
       <c r="AB83" s="38"/>
       <c r="AC83" s="41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:29" ht="24" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B84" s="37" t="s">
         <v>189</v>
       </c>
@@ -6912,7 +6804,7 @@
         <v>6</v>
       </c>
       <c r="D84" s="38">
-        <v>2009</v>
+        <v>1997</v>
       </c>
       <c r="E84" s="38"/>
       <c r="G84" s="39"/>
@@ -6937,21 +6829,43 @@
       <c r="AA84" s="38"/>
       <c r="AB84" s="38"/>
       <c r="AC84" s="41" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>162</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="D85" s="11">
-        <v>2011</v>
-      </c>
-      <c r="AC85" s="23" t="s">
-        <v>150</v>
+      <c r="B85" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C85" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="38">
+        <v>2001</v>
+      </c>
+      <c r="E85" s="38"/>
+      <c r="G85" s="39"/>
+      <c r="H85" s="38"/>
+      <c r="I85" s="40"/>
+      <c r="J85" s="38"/>
+      <c r="K85" s="38"/>
+      <c r="L85" s="39"/>
+      <c r="M85" s="38"/>
+      <c r="N85" s="38"/>
+      <c r="O85" s="38"/>
+      <c r="P85" s="38"/>
+      <c r="Q85" s="38"/>
+      <c r="R85" s="38"/>
+      <c r="S85" s="38"/>
+      <c r="T85" s="38"/>
+      <c r="U85" s="40"/>
+      <c r="V85" s="38"/>
+      <c r="X85" s="38"/>
+      <c r="Y85" s="38"/>
+      <c r="Z85" s="38"/>
+      <c r="AA85" s="38"/>
+      <c r="AB85" s="38"/>
+      <c r="AC85" s="41" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.25">
@@ -6959,10 +6873,10 @@
         <v>189</v>
       </c>
       <c r="C86" s="38" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D86" s="38">
-        <v>1997</v>
+        <v>2004</v>
       </c>
       <c r="E86" s="38"/>
       <c r="G86" s="39"/>
@@ -6986,19 +6900,20 @@
       <c r="Z86" s="38"/>
       <c r="AA86" s="38"/>
       <c r="AB86" s="38"/>
-      <c r="AC86" s="42" t="s">
-        <v>19</v>
+      <c r="AC86" s="41" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:29" ht="24" x14ac:dyDescent="0.25">
+      <c r="A87" s="51"/>
       <c r="B87" s="37" t="s">
         <v>189</v>
       </c>
       <c r="C87" s="38" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D87" s="38">
-        <v>1997</v>
+        <v>2004</v>
       </c>
       <c r="E87" s="38"/>
       <c r="G87" s="39"/>
@@ -7022,16 +6937,17 @@
       <c r="Z87" s="38"/>
       <c r="AA87" s="38"/>
       <c r="AB87" s="38"/>
-      <c r="AC87" s="42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC87" s="41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" ht="24" x14ac:dyDescent="0.25">
+      <c r="A88" s="51"/>
       <c r="B88" s="37" t="s">
         <v>189</v>
       </c>
       <c r="C88" s="38" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D88" s="38">
         <v>2004</v>
@@ -7058,64 +6974,155 @@
       <c r="Z88" s="38"/>
       <c r="AA88" s="38"/>
       <c r="AB88" s="38"/>
-      <c r="AC88" s="42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>162</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D89" s="11">
-        <v>2007</v>
-      </c>
-      <c r="AC89" s="52" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>162</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D90" s="11">
-        <v>2012</v>
-      </c>
-      <c r="AC90" s="52" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>162</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="D91" s="11">
-        <v>2012</v>
-      </c>
-      <c r="AC91" s="23" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>162</v>
-      </c>
-      <c r="C92" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D92" s="11">
-        <v>2004</v>
-      </c>
-      <c r="AC92" s="23" t="s">
-        <v>154</v>
+      <c r="AC88" s="41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29" ht="24" x14ac:dyDescent="0.25">
+      <c r="A89" s="51"/>
+      <c r="B89" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C89" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="38">
+        <v>2005</v>
+      </c>
+      <c r="E89" s="38"/>
+      <c r="G89" s="39"/>
+      <c r="H89" s="38"/>
+      <c r="I89" s="40"/>
+      <c r="J89" s="38"/>
+      <c r="K89" s="38"/>
+      <c r="L89" s="39"/>
+      <c r="M89" s="38"/>
+      <c r="N89" s="38"/>
+      <c r="O89" s="38"/>
+      <c r="P89" s="38"/>
+      <c r="Q89" s="38"/>
+      <c r="R89" s="38"/>
+      <c r="S89" s="38"/>
+      <c r="T89" s="38"/>
+      <c r="U89" s="40"/>
+      <c r="V89" s="38"/>
+      <c r="X89" s="38"/>
+      <c r="Y89" s="38"/>
+      <c r="Z89" s="38"/>
+      <c r="AA89" s="38"/>
+      <c r="AB89" s="38"/>
+      <c r="AC89" s="41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29" ht="24" x14ac:dyDescent="0.25">
+      <c r="A90" s="51"/>
+      <c r="B90" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C90" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="38">
+        <v>2008</v>
+      </c>
+      <c r="E90" s="38"/>
+      <c r="G90" s="39"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="40"/>
+      <c r="J90" s="38"/>
+      <c r="K90" s="38"/>
+      <c r="L90" s="39"/>
+      <c r="M90" s="38"/>
+      <c r="N90" s="38"/>
+      <c r="O90" s="38"/>
+      <c r="P90" s="38"/>
+      <c r="Q90" s="38"/>
+      <c r="R90" s="38"/>
+      <c r="S90" s="38"/>
+      <c r="T90" s="38"/>
+      <c r="U90" s="40"/>
+      <c r="V90" s="38"/>
+      <c r="X90" s="38"/>
+      <c r="Y90" s="38"/>
+      <c r="Z90" s="38"/>
+      <c r="AA90" s="38"/>
+      <c r="AB90" s="38"/>
+      <c r="AC90" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" ht="24" x14ac:dyDescent="0.25">
+      <c r="A91" s="51"/>
+      <c r="B91" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C91" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="38">
+        <v>2009</v>
+      </c>
+      <c r="E91" s="38"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="38"/>
+      <c r="I91" s="40"/>
+      <c r="J91" s="38"/>
+      <c r="K91" s="38"/>
+      <c r="L91" s="39"/>
+      <c r="M91" s="38"/>
+      <c r="N91" s="38"/>
+      <c r="O91" s="38"/>
+      <c r="P91" s="38"/>
+      <c r="Q91" s="38"/>
+      <c r="R91" s="38"/>
+      <c r="S91" s="38"/>
+      <c r="T91" s="38"/>
+      <c r="U91" s="40"/>
+      <c r="V91" s="38"/>
+      <c r="X91" s="38"/>
+      <c r="Y91" s="38"/>
+      <c r="Z91" s="38"/>
+      <c r="AA91" s="38"/>
+      <c r="AB91" s="38"/>
+      <c r="AC91" s="41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" ht="24" x14ac:dyDescent="0.25">
+      <c r="B92" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C92" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="38">
+        <v>2009</v>
+      </c>
+      <c r="E92" s="38"/>
+      <c r="G92" s="39"/>
+      <c r="H92" s="38"/>
+      <c r="I92" s="40"/>
+      <c r="J92" s="38"/>
+      <c r="K92" s="38"/>
+      <c r="L92" s="39"/>
+      <c r="M92" s="38"/>
+      <c r="N92" s="38"/>
+      <c r="O92" s="38"/>
+      <c r="P92" s="38"/>
+      <c r="Q92" s="38"/>
+      <c r="R92" s="38"/>
+      <c r="S92" s="38"/>
+      <c r="T92" s="38"/>
+      <c r="U92" s="40"/>
+      <c r="V92" s="38"/>
+      <c r="X92" s="38"/>
+      <c r="Y92" s="38"/>
+      <c r="Z92" s="38"/>
+      <c r="AA92" s="38"/>
+      <c r="AB92" s="38"/>
+      <c r="AC92" s="41" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.25">
@@ -7123,10 +7130,10 @@
         <v>189</v>
       </c>
       <c r="C93" s="38" t="s">
-        <v>116</v>
+        <v>21</v>
       </c>
       <c r="D93" s="38">
-        <v>2004</v>
+        <v>1997</v>
       </c>
       <c r="E93" s="38"/>
       <c r="G93" s="39"/>
@@ -7150,19 +7157,19 @@
       <c r="Z93" s="38"/>
       <c r="AA93" s="38"/>
       <c r="AB93" s="38"/>
-      <c r="AC93" s="43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC93" s="42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" ht="24" x14ac:dyDescent="0.25">
       <c r="B94" s="37" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C94" s="38" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="D94" s="38">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="E94" s="38"/>
       <c r="G94" s="39"/>
@@ -7186,254 +7193,310 @@
       <c r="Z94" s="38"/>
       <c r="AA94" s="38"/>
       <c r="AB94" s="38"/>
-      <c r="AC94" s="58" t="s">
-        <v>126</v>
+      <c r="AC94" s="42" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>162</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="D95" s="11">
-        <v>2012</v>
-      </c>
-      <c r="AC95" s="23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="96" spans="1:29" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>316</v>
-      </c>
-      <c r="C96" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="D96" s="11">
+      <c r="B95" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C95" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D95" s="38">
+        <v>2004</v>
+      </c>
+      <c r="E95" s="38"/>
+      <c r="G95" s="39"/>
+      <c r="H95" s="38"/>
+      <c r="I95" s="40"/>
+      <c r="J95" s="38"/>
+      <c r="K95" s="38"/>
+      <c r="L95" s="39"/>
+      <c r="M95" s="38"/>
+      <c r="N95" s="38"/>
+      <c r="O95" s="38"/>
+      <c r="P95" s="38"/>
+      <c r="Q95" s="38"/>
+      <c r="R95" s="38"/>
+      <c r="S95" s="38"/>
+      <c r="T95" s="38"/>
+      <c r="U95" s="40"/>
+      <c r="V95" s="38"/>
+      <c r="X95" s="38"/>
+      <c r="Y95" s="38"/>
+      <c r="Z95" s="38"/>
+      <c r="AA95" s="38"/>
+      <c r="AB95" s="38"/>
+      <c r="AC95" s="42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B96" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C96" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D96" s="38">
+        <v>2004</v>
+      </c>
+      <c r="E96" s="38"/>
+      <c r="G96" s="39"/>
+      <c r="H96" s="38"/>
+      <c r="I96" s="40"/>
+      <c r="J96" s="38"/>
+      <c r="K96" s="38"/>
+      <c r="L96" s="39"/>
+      <c r="M96" s="38"/>
+      <c r="N96" s="38"/>
+      <c r="O96" s="38"/>
+      <c r="P96" s="38"/>
+      <c r="Q96" s="38"/>
+      <c r="R96" s="38"/>
+      <c r="S96" s="38"/>
+      <c r="T96" s="38"/>
+      <c r="U96" s="40"/>
+      <c r="V96" s="38"/>
+      <c r="X96" s="38"/>
+      <c r="Y96" s="38"/>
+      <c r="Z96" s="38"/>
+      <c r="AA96" s="38"/>
+      <c r="AB96" s="38"/>
+      <c r="AC96" s="43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A97" s="51"/>
+      <c r="B97" s="51" t="s">
+        <v>264</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D97" s="11">
+        <v>2011</v>
+      </c>
+      <c r="AC97" s="58" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>264</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D98" s="11">
+        <v>2015</v>
+      </c>
+      <c r="AC98" s="58" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>264</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D99" s="11">
         <v>2014</v>
       </c>
-      <c r="M96" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="W96" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="AC96" s="50" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="97" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>162</v>
-      </c>
-      <c r="C97" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D97" s="11">
-        <v>2003</v>
-      </c>
-      <c r="AC97" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="98" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>162</v>
-      </c>
-      <c r="C98" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D98" s="11">
-        <v>2007</v>
-      </c>
-      <c r="AC98" s="23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="99" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="C99" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D99" s="11">
-        <v>2011</v>
-      </c>
       <c r="AC99" s="50" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="100" spans="2:29" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>264</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D100" s="11">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="AC100" s="50" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="101" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>335</v>
-      </c>
-      <c r="C101" s="11" t="s">
-        <v>334</v>
-      </c>
-      <c r="D101" s="11">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B101" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="C101" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="D101" s="38">
+        <v>2012</v>
+      </c>
+      <c r="E101" s="38"/>
+      <c r="G101" s="39"/>
+      <c r="H101" s="38"/>
+      <c r="I101" s="40"/>
+      <c r="J101" s="38"/>
+      <c r="K101" s="38"/>
+      <c r="L101" s="39"/>
+      <c r="M101" s="38"/>
+      <c r="N101" s="38"/>
+      <c r="O101" s="38"/>
+      <c r="P101" s="38"/>
+      <c r="Q101" s="38"/>
+      <c r="R101" s="38"/>
+      <c r="S101" s="38"/>
+      <c r="T101" s="38"/>
+      <c r="U101" s="40"/>
+      <c r="V101" s="38"/>
+      <c r="X101" s="38"/>
+      <c r="Y101" s="38"/>
+      <c r="Z101" s="38"/>
+      <c r="AA101" s="38"/>
+      <c r="AB101" s="38"/>
+      <c r="AC101" s="57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A102" s="51"/>
+      <c r="B102" s="51"/>
+      <c r="C102" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D102" s="11">
+        <v>2013</v>
+      </c>
+      <c r="AC102" s="58" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A103" s="51"/>
+      <c r="B103" s="51"/>
+      <c r="C103" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D103" s="11">
+        <v>2016</v>
+      </c>
+      <c r="AC103" s="58" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A104" s="51"/>
+      <c r="B104" s="51"/>
+      <c r="C104" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D104" s="11">
+        <v>2011</v>
+      </c>
+      <c r="AC104" s="58" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C105" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D105" s="11">
+        <v>2013</v>
+      </c>
+      <c r="AC105" s="50" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A106" s="51"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="D106" s="11">
         <v>2009</v>
       </c>
-      <c r="AC101" s="50" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="102" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>162</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="D102" s="11">
-        <v>2012</v>
-      </c>
-      <c r="AC102" s="23" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="103" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>162</v>
-      </c>
-      <c r="C103" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="D103" s="11">
-        <v>2008</v>
-      </c>
-      <c r="AC103" s="23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="104" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>264</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="D104" s="11">
-        <v>2012</v>
-      </c>
-      <c r="AC104" s="50" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="105" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>271</v>
-      </c>
-      <c r="C105" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="D105" s="11">
-        <v>2014</v>
-      </c>
-      <c r="AC105" s="50" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="106" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="C106" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="D106" s="11">
-        <v>2011</v>
-      </c>
-      <c r="AC106" s="50" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="107" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>162</v>
-      </c>
+      <c r="AC106" s="58" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A107" s="51"/>
+      <c r="B107" s="51"/>
       <c r="C107" s="11" t="s">
-        <v>118</v>
+        <v>232</v>
       </c>
       <c r="D107" s="11">
-        <v>2006</v>
-      </c>
-      <c r="AC107" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="108" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>162</v>
-      </c>
+        <v>2009</v>
+      </c>
+      <c r="AC107" s="58" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A108" s="51"/>
+      <c r="B108" s="51"/>
       <c r="C108" s="11" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
       <c r="D108" s="11">
         <v>2012</v>
       </c>
-      <c r="AC108" s="23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="109" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>271</v>
-      </c>
+      <c r="AC108" s="58" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A109" s="59"/>
+      <c r="B109" s="51"/>
       <c r="C109" s="11" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="D109" s="11">
-        <v>2012</v>
-      </c>
-      <c r="AC109" s="50" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="110" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>162</v>
-      </c>
+        <v>2015</v>
+      </c>
+      <c r="AC109" s="58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C110" s="11" t="s">
-        <v>186</v>
+        <v>117</v>
       </c>
       <c r="D110" s="11">
-        <v>2006</v>
-      </c>
-      <c r="AC110" s="23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="111" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>162</v>
-      </c>
+        <v>2011</v>
+      </c>
+      <c r="AC110" s="50" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C111" s="11" t="s">
-        <v>187</v>
+        <v>238</v>
       </c>
       <c r="D111" s="11">
-        <v>2009</v>
-      </c>
-      <c r="AC111" s="23" t="s">
-        <v>161</v>
+        <v>2011</v>
+      </c>
+      <c r="AC111" s="50" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="113" spans="29:29" x14ac:dyDescent="0.25">
+      <c r="AC113" s="50" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AC111">
-    <sortCondition ref="E2:E111"/>
-    <sortCondition ref="C2:C111"/>
-    <sortCondition ref="D2:D111"/>
-    <sortCondition ref="B2:B111"/>
+  <sortState ref="A2:AC113">
+    <sortCondition ref="E2:E113"/>
+    <sortCondition ref="B2:B113"/>
+    <sortCondition ref="C2:C113"/>
+    <sortCondition ref="D2:D113"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">

</xml_diff>